<commit_message>
tables created in excel and read to jason seperately
</commit_message>
<xml_diff>
--- a/labShop/src/main/resources/labshop.xlsx
+++ b/labShop/src/main/resources/labshop.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="detailorder" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>a</t>
   </si>
@@ -39,40 +39,94 @@
     <t>f</t>
   </si>
   <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>cb</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>db</t>
-  </si>
-  <si>
-    <t>ea</t>
-  </si>
-  <si>
-    <t>eb</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>fb</t>
+    <t>ردیف</t>
+  </si>
+  <si>
+    <t>نام محصول</t>
+  </si>
+  <si>
+    <t>واحد</t>
+  </si>
+  <si>
+    <t>تعداد</t>
+  </si>
+  <si>
+    <t>فی</t>
+  </si>
+  <si>
+    <t>تخفیف</t>
+  </si>
+  <si>
+    <t>قیمت</t>
+  </si>
+  <si>
+    <t>نام تامین کننده</t>
+  </si>
+  <si>
+    <t>تاریخ</t>
+  </si>
+  <si>
+    <t>نحوه تسویه حساب</t>
+  </si>
+  <si>
+    <t>تحفیف فاکتور</t>
+  </si>
+  <si>
+    <t>قیمت کل</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1397-10-23</t>
+  </si>
+  <si>
+    <t>akbari</t>
+  </si>
+  <si>
+    <t>naghd</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>totalPrice</t>
   </si>
 </sst>
 </file>
@@ -125,6 +179,40 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="detailorder" displayName="detailorder" ref="A1:G8" totalsRowShown="0">
+  <autoFilter ref="A1:G8"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="row"/>
+    <tableColumn id="2" name="product"/>
+    <tableColumn id="3" name="unit"/>
+    <tableColumn id="4" name="qty"/>
+    <tableColumn id="5" name="fee"/>
+    <tableColumn id="6" name="discount"/>
+    <tableColumn id="7" name="price">
+      <calculatedColumnFormula>IF(F2="-",E2*D2,D2*E2*(1-F2))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="order" displayName="order" ref="K1:O2" totalsRowShown="0">
+  <autoFilter ref="K1:O2"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="date"/>
+    <tableColumn id="2" name="supplier"/>
+    <tableColumn id="3" name="payment"/>
+    <tableColumn id="4" name="discount"/>
+    <tableColumn id="5" name="totalPrice">
+      <calculatedColumnFormula>SUM(G2:G8)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,175 +478,285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.19921875" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="13.59765625" customWidth="1"/>
+    <col min="14" max="14" width="10.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>1500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <f>IF(F2="-",E2*D2,D2*E2*(1-F2))</f>
+        <v>150000</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>SUM(G2:G8)</f>
+        <v>356200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1500</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="0">IF(F3="-",E3*D3,D3*E3*(1-F3))</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>450</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E5">
+        <v>7000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>2000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>140000</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>350</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
core service and json Deserializer package completed
</commit_message>
<xml_diff>
--- a/labShop/src/main/resources/labshop.xlsx
+++ b/labShop/src/main/resources/labshop.xlsx
@@ -19,95 +19,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>ردیف</t>
-  </si>
-  <si>
-    <t>نام محصول</t>
-  </si>
-  <si>
-    <t>واحد</t>
-  </si>
-  <si>
-    <t>تعداد</t>
-  </si>
-  <si>
-    <t>فی</t>
-  </si>
-  <si>
-    <t>تخفیف</t>
-  </si>
-  <si>
-    <t>قیمت</t>
-  </si>
-  <si>
-    <t>نام تامین کننده</t>
-  </si>
-  <si>
-    <t>تاریخ</t>
-  </si>
-  <si>
-    <t>نحوه تسویه حساب</t>
-  </si>
-  <si>
-    <t>تحفیف فاکتور</t>
-  </si>
-  <si>
-    <t>قیمت کل</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>1397-10-23</t>
-  </si>
-  <si>
-    <t>akbari</t>
-  </si>
-  <si>
-    <t>naghd</t>
-  </si>
-  <si>
     <t>row</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
-    <t>qty</t>
-  </si>
-  <si>
     <t>fee</t>
   </si>
   <si>
@@ -120,13 +42,34 @@
     <t>date</t>
   </si>
   <si>
-    <t>supplier</t>
-  </si>
-  <si>
-    <t>payment</t>
-  </si>
-  <si>
     <t>totalPrice</t>
+  </si>
+  <si>
+    <t>supplierId</t>
+  </si>
+  <si>
+    <t>paymentType</t>
+  </si>
+  <si>
+    <t>orderDiscount</t>
+  </si>
+  <si>
+    <t>productId</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>addad</t>
+  </si>
+  <si>
+    <t>basteh</t>
+  </si>
+  <si>
+    <t>karton</t>
   </si>
 </sst>
 </file>
@@ -162,13 +105,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -186,13 +134,13 @@
   <autoFilter ref="A1:G8"/>
   <tableColumns count="7">
     <tableColumn id="1" name="row"/>
-    <tableColumn id="2" name="product"/>
+    <tableColumn id="2" name="productId"/>
     <tableColumn id="3" name="unit"/>
-    <tableColumn id="4" name="qty"/>
+    <tableColumn id="4" name="quantity"/>
     <tableColumn id="5" name="fee"/>
     <tableColumn id="6" name="discount"/>
     <tableColumn id="7" name="price">
-      <calculatedColumnFormula>IF(F2="-",E2*D2,D2*E2*(1-F2))</calculatedColumnFormula>
+      <calculatedColumnFormula>TEXT(IF(F2="-",E2*D2,D2*E2*(1-F2)),"0")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -203,13 +151,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="order" displayName="order" ref="K1:O2" totalsRowShown="0">
   <autoFilter ref="K1:O2"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="date"/>
-    <tableColumn id="2" name="supplier"/>
-    <tableColumn id="3" name="payment"/>
-    <tableColumn id="4" name="discount"/>
-    <tableColumn id="5" name="totalPrice">
-      <calculatedColumnFormula>SUM(G2:G8)</calculatedColumnFormula>
+    <tableColumn id="1" name="date" dataDxfId="0">
+      <calculatedColumnFormula>TEXT(J2,"yyyy-MM-dd")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="2" name="supplierId"/>
+    <tableColumn id="3" name="paymentType"/>
+    <tableColumn id="4" name="orderDiscount"/>
+    <tableColumn id="5" name="totalPrice"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -478,15 +426,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.19921875" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="10" max="11" width="9.8984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="13.59765625" customWidth="1"/>
     <col min="14" max="14" width="10.59765625" customWidth="1"/>
@@ -494,51 +443,51 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -547,38 +496,41 @@
         <v>1500</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2">
-        <f>IF(F2="-",E2*D2,D2*E2*(1-F2))</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>TEXT(IF(F2="-",E2*D2,D2*E2*(1-F2)),"0")</f>
         <v>150000</v>
       </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
+      <c r="J2" s="1">
+        <v>43758</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>TEXT(J2,"yyyy-MM-dd")</f>
+        <v>2019-10-20</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <f>SUM(G2:G8)</f>
-        <v>356200</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -587,10 +539,10 @@
         <v>1500</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">IF(F3="-",E3*D3,D3*E3*(1-F3))</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G8" si="0">TEXT(IF(F3="-",E3*D3,D3*E3*(1-F3)),"0")</f>
         <v>30000</v>
       </c>
     </row>
@@ -598,11 +550,11 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4">
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -611,9 +563,9 @@
         <v>450</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
@@ -622,11 +574,11 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -635,9 +587,9 @@
         <v>7000</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>28000</v>
       </c>
@@ -646,11 +598,11 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6">
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>70</v>
@@ -659,37 +611,22 @@
         <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>140000</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+      <c r="B7">
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -698,9 +635,9 @@
         <v>350</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>3500</v>
       </c>
@@ -709,11 +646,11 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
+      <c r="B8">
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -722,41 +659,19 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>